<commit_message>
TPS reports fully functional
</commit_message>
<xml_diff>
--- a/tps/inputs/TEMPLATE_DISTRATOR.xlsx
+++ b/tps/inputs/TEMPLATE_DISTRATOR.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-audrs\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Lins\Desktop\v5\tps\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC7A9286-AFB8-4F45-9A45-BC25CE17899B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC29C24-3DA2-483E-BB03-58FA6F3FEC3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="2400" windowWidth="20715" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFORMANCE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PERFORMANCE!$A:$I</definedName>
     <definedName name="BillName">PERFORMANCE!#REF!</definedName>
     <definedName name="ColumnTitle1">#REF!</definedName>
     <definedName name="ColumnTitleRegion1..G6.1">PERFORMANCE!#REF!</definedName>
@@ -24,21 +23,20 @@
     <definedName name="CustomerLookup">#REF!</definedName>
     <definedName name="Deposit">PERFORMANCE!#REF!</definedName>
     <definedName name="InvoiceSubtotal">PERFORMANCE!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PERFORMANCE!$A:$I</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">PERFORMANCE!#REF!</definedName>
     <definedName name="RowTitleRegion1..H3">PERFORMANCE!$G$3</definedName>
     <definedName name="RowTitleRegion2..C8">PERFORMANCE!#REF!</definedName>
     <definedName name="RowTitleRegion3..E8">PERFORMANCE!#REF!</definedName>
     <definedName name="RowTitleRegion4..H18">PERFORMANCE!#REF!</definedName>
     <definedName name="Title2">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">PERFORMANCE!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>NOME</t>
   </si>
@@ -96,34 +94,7 @@
     <t>E</t>
   </si>
   <si>
-    <t xml:space="preserve">      Q. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q. 10</t>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -137,7 +108,7 @@
     <numFmt numFmtId="167" formatCode="00000"/>
     <numFmt numFmtId="168" formatCode="[&lt;=9999999]###\-####;###\-###\-####"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3"/>
@@ -306,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -400,17 +371,6 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -464,19 +424,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -560,7 +507,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -579,19 +526,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -633,7 +571,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -642,14 +580,11 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -657,16 +592,13 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -678,33 +610,36 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
+    <cellStyle name="Accent1" xfId="12" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Bottom Border" xfId="24" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma" xfId="7" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="8" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="9" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="10" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Date" xfId="15" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Ênfase1" xfId="12" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="16" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Invoice description" xfId="21" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Invoice no. &amp; contact info" xfId="22" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Left Align" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Moeda" xfId="9" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Moeda [0]" xfId="10" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="11" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Phone" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Porcentagem" xfId="11" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Right Align" xfId="14" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="Right Indent" xfId="25" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Separador de milhares [0]" xfId="8" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="16" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Top align" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vírgula" xfId="7" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Zip Code" xfId="19" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="znavigation cells" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
   </cellStyles>
@@ -898,7 +833,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1FD4469-38C1-4A3D-A0A2-66BEA12DD7B8}"/>
@@ -1161,13 +1096,13 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="5" width="15" customWidth="1"/>
@@ -1178,25 +1113,25 @@
     <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1"/>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="26"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="34" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="24" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
@@ -1206,96 +1141,96 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1">
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="25"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="B5" s="12"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="38" t="s">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="22"/>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="B6" s="23"/>
-      <c r="C6" s="31" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1">
-      <c r="B8" s="24"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1">
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="21"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="25"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1">
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="3"/>
@@ -1303,157 +1238,130 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1">
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1">
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1">
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1">
+    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="30" customHeight="1">
+    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1">
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1">
+    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" ht="30" customHeight="1">
+    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1">
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="30" customHeight="1">
+    <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1465,7 +1373,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="30" customHeight="1">
+    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1477,7 +1385,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="30" customHeight="1">
+    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1489,7 +1397,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1">
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1501,7 +1409,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1">
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1513,7 +1421,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="30" customHeight="1">
+    <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1525,7 +1433,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1">
+    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1537,7 +1445,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1">
+    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1549,7 +1457,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1">
+    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1561,7 +1469,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1">
+    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1573,7 +1481,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1">
+    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1585,7 +1493,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1597,7 +1505,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="1:11" ht="30" customHeight="1">
+    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1609,7 +1517,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" ht="30" customHeight="1">
+    <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1621,7 +1529,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="1:11" ht="30" customHeight="1">
+    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1633,7 +1541,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" ht="30" customHeight="1">
+    <row r="36" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1645,7 +1553,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1">
+    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1657,7 +1565,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11" ht="30" customHeight="1">
+    <row r="38" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1669,7 +1577,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="1:11" ht="30" customHeight="1">
+    <row r="39" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1681,7 +1589,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" ht="30" customHeight="1">
+    <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1693,7 +1601,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1">
+    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1705,7 +1613,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1">
+    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1717,7 +1625,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" ht="30" customHeight="1">
+    <row r="43" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1729,7 +1637,7 @@
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" ht="30" customHeight="1">
+    <row r="44" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1741,7 +1649,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1">
+    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1752,114 +1660,6 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" ht="30" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:11" ht="30" customHeight="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-    </row>
-    <row r="48" spans="1:11" ht="30" customHeight="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-    </row>
-    <row r="49" spans="1:11" ht="30" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:11" ht="30" customHeight="1">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-    </row>
-    <row r="51" spans="1:11" ht="30" customHeight="1">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:11" ht="30" customHeight="1">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-    </row>
-    <row r="53" spans="1:11" ht="30" customHeight="1">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:11" ht="30" customHeight="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" sort="0"/>
@@ -1921,9 +1721,6 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="872" yWindow="452" count="8">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select customer name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" prompt="Select customer name in this cell. Press ALT+DOWN ARROW to open drop-down list, then ENTER to make selection. Add more customers to Customers worksheet to expand selection list" sqref="B9:B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>CustomerLookup</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create Service Invoice in this workbook. Enter company &amp; invoice details in this worksheet, &amp; customer details in Customers worksheet. Select cell J1 to navigate to Customers worksheet" sqref="A3" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter company name in below cell. Enter Invoice Number, Invoice Date and Date Due in cells H1, H2 and H3" sqref="B4:B5" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Customer Phone number is automatically updated in cell at right" sqref="C9 C10" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
@@ -1931,6 +1728,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Customers worksheet. This cell will not print" sqref="J3" xr:uid="{00000000-0002-0000-0000-000030000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Invoice Date in cell at right" sqref="G4:G7" xr:uid="{00000000-0002-0000-0000-000019000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter invoicing company email address in this cell" sqref="D5 B3 E7:F7 B7:C7 B6:G6 C3 G3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select customer name from the list. Select CANCEL, then press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" prompt="Select customer name in this cell. Press ALT+DOWN ARROW to open drop-down list, then ENTER to make selection. Add more customers to Customers worksheet to expand selection list" sqref="B9:B11" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>CustomerLookup</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="J3" location="Customers!A1" tooltip="Select to navigate to Customers worksheet" display="Customers" xr:uid="{00000000-0004-0000-0000-000004000000}"/>

</xml_diff>